<commit_message>
Assembled table of comparable surface complexation results
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SurfaceComplRxns.xlsx
+++ b/Manuscript/Tables/SurfaceComplRxns.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
-  <si>
-    <t>Reactions and log Kd</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Ferrihydrite</t>
   </si>
@@ -105,6 +102,51 @@
   </si>
   <si>
     <t>Data Fitting, Pyrite sites by Naveau, 2006</t>
+  </si>
+  <si>
+    <t>Simple Models</t>
+  </si>
+  <si>
+    <t>Advanced Models</t>
+  </si>
+  <si>
+    <t>4 FhyOH + Ra+2 = (FhyOH)3FhyORa+ + H+</t>
+  </si>
+  <si>
+    <t>4 FhyOH + Ra+2 + 2 H+ = (FhyOH2)2(FhyOH)2Ra+4</t>
+  </si>
+  <si>
+    <t>Data fitting</t>
+  </si>
+  <si>
+    <t>NaMont</t>
+  </si>
+  <si>
+    <t>Clay_wOH + H+ = Clay_wOH2+</t>
+  </si>
+  <si>
+    <t>Clay_wOH = Clay_wO- + H+</t>
+  </si>
+  <si>
+    <t>Clay_sOH + H+ = Clay_sOH2+</t>
+  </si>
+  <si>
+    <t>Clay_sOH = Clay_sO- + H+</t>
+  </si>
+  <si>
+    <t>Clay_sOH + Ra+2 = Clay_sOHRa+2</t>
+  </si>
+  <si>
+    <t>Clay_wOH + Ra+2 = Clay_wORa+ + H+</t>
+  </si>
+  <si>
+    <t>Reactions and log Kd (Table 2)</t>
+  </si>
+  <si>
+    <t>4 GoeOH + Ra+2 = (GoeOH)3(GoeO)Ra+ + H+</t>
+  </si>
+  <si>
+    <t>4 GoeOH + Ra+2 = (GoeOH)4Ra+2</t>
   </si>
 </sst>
 </file>
@@ -140,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,202 +465,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7.92</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>-8.93</v>
+        <v>7.92</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5">
+        <v>-8.93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>5.7</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <f>0.00005/0.03</f>
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>4.8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>-10.4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
+        <v>4.8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-10.4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>3.5</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <f>0.000011/0.03</f>
         <v>3.6666666666666667E-4</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
+      <c r="B14">
         <v>0.15</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <f>0.0000253/0.03</f>
         <v>8.433333333333333E-4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4.5</v>
+      </c>
+      <c r="D15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>4.5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B16">
+        <v>-7.9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>-7.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
+      <c r="B17">
         <v>6.4</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <f>0.0000002/0.03</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B20">
+        <v>6.45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
-        <v>6.45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
+      <c r="B21">
         <v>-6.4</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <f>0.000000892/0.04</f>
         <v>2.23E-5</v>
       </c>
-      <c r="D17" t="s">
-        <v>26</v>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>7.92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>-8.93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>-1.4</v>
+      </c>
+      <c r="C27" s="1">
+        <f>0.0000525/0.03</f>
+        <v>1.75E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>7.92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>-8.93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>-5</v>
+      </c>
+      <c r="C33">
+        <f>0.000011/0.03</f>
+        <v>3.6666666666666667E-4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>0.15</v>
+      </c>
+      <c r="C37">
+        <f>0.0000253/0.03</f>
+        <v>8.433333333333333E-4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>4.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39">
+        <v>-7.9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>4.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41">
+        <v>-7.9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>0.000000006/0.03</f>
+        <v>2.0000000000000002E-7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>7.5</v>
+      </c>
+      <c r="C43">
+        <f>0.000000019/0.03</f>
+        <v>6.3333333333333345E-7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerunning Surface Complex models with real surface areas, still need to do goethite SSM and Mont
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SurfaceComplRxns.xlsx
+++ b/Manuscript/Tables/SurfaceComplRxns.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Ferrihydrite</t>
   </si>
@@ -116,9 +116,6 @@
     <t>4 FhyOH + Ra+2 + 2 H+ = (FhyOH2)2(FhyOH)2Ra+4</t>
   </si>
   <si>
-    <t>Data fitting</t>
-  </si>
-  <si>
     <t>NaMont</t>
   </si>
   <si>
@@ -147,6 +144,18 @@
   </si>
   <si>
     <t>Reactions and log K (Table 2)</t>
+  </si>
+  <si>
+    <t>SA (m2/g)</t>
+  </si>
+  <si>
+    <t>Data Fitting, Sites for Sajih</t>
+  </si>
+  <si>
+    <t>Data fitting, Sajih sites</t>
+  </si>
+  <si>
+    <t>Data fitting, Sajih Sites</t>
   </si>
 </sst>
 </file>
@@ -465,366 +474,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5">
+        <f>0.000056/0.03</f>
+        <v>1.8666666666666666E-3</v>
+      </c>
+      <c r="E5">
+        <v>382.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>7.92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>-8.93</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>5.7</v>
       </c>
-      <c r="C6">
-        <f>0.00005/0.03</f>
-        <v>1.6666666666666668E-3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>4.8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>-10.4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>3.5</v>
-      </c>
-      <c r="C11">
+      <c r="C10">
         <f>0.000011/0.03</f>
         <v>3.6666666666666667E-4</v>
       </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>4.8</v>
+      </c>
       <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>-10.4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>3.5</v>
+      </c>
+      <c r="D13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>0.15</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <f>0.0000253/0.03</f>
         <v>8.433333333333333E-4</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>4.5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>-7.9</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>6.4</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <f>0.0000002/0.03</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>6.45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>-6.4</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <f>0.000000892/0.04</f>
         <v>2.23E-5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>7.92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>-8.93</v>
-      </c>
-      <c r="D26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>-1.4</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="C26" s="1">
         <f>0.0000525/0.03</f>
         <v>1.75E-3</v>
       </c>
+      <c r="E26">
+        <v>382.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>7.92</v>
+      </c>
       <c r="D27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>-8.93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>-1.4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>0</v>
       </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <v>7.92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32">
-        <v>-8.93</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
+      <c r="C32" s="1">
+        <f>0.00000192/0.03</f>
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="E32">
+        <v>146.46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B33">
-        <v>-5</v>
-      </c>
-      <c r="C33">
-        <f>0.000011/0.03</f>
-        <v>3.6666666666666667E-4</v>
+        <v>4.8</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>4.9000000000000004</v>
+        <v>-10.4</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>-2.9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>0.15</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <f>0.0000253/0.03</f>
         <v>8.433333333333333E-4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D39" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38">
-        <v>4.5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39">
-        <v>-7.9</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B40">
         <v>4.5</v>
@@ -835,7 +838,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B41">
         <v>-7.9</v>
@@ -846,31 +849,53 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B42">
+        <v>4.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43">
+        <v>-7.9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44">
         <v>0</v>
       </c>
-      <c r="C42">
+      <c r="C44">
         <f>0.000000006/0.03</f>
         <v>2.0000000000000002E-7</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45">
         <v>7.5</v>
       </c>
-      <c r="C43">
+      <c r="C45">
         <f>0.000000019/0.03</f>
         <v>6.3333333333333345E-7</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished rerun of SCM with measured SA
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SurfaceComplRxns.xlsx
+++ b/Manuscript/Tables/SurfaceComplRxns.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Ferrihydrite</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Data fitting, Sajih Sites</t>
+  </si>
+  <si>
+    <t>Real surface area with site density from Sverjensky, 2006</t>
+  </si>
+  <si>
+    <t>calculated mol/g from sverjensky</t>
+  </si>
+  <si>
+    <t>Data fitting, Reported CEC by Clays.Org, Constant fitted</t>
+  </si>
+  <si>
+    <t>ClayO- + Ra+2 = ClayORa+</t>
+  </si>
+  <si>
+    <t>Constants and Sites from Data Fitting</t>
+  </si>
+  <si>
+    <t>Data Fitting, sites also by data fitting</t>
   </si>
 </sst>
 </file>
@@ -474,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,21 +503,21 @@
     <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -513,7 +531,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -525,7 +543,7 @@
         <v>382.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -536,7 +554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -547,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -558,16 +576,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="C10">
-        <f>0.000011/0.03</f>
-        <v>3.6666666666666667E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <f>0.00012/0.03</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>146.46</v>
+      </c>
+      <c r="F10">
+        <f>146.46*16.4*10^18/6.022E+23</f>
+        <v>3.9886150780471599E-3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -578,7 +609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -589,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -600,12 +631,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -617,7 +648,10 @@
         <v>8.433333333333333E-4</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>46</v>
+      </c>
+      <c r="E16">
+        <v>50.161999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -647,81 +681,78 @@
         <v>14</v>
       </c>
       <c r="B19">
-        <v>6.4</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C19">
-        <f>0.0000002/0.03</f>
-        <v>6.6666666666666666E-6</v>
+        <f>0.0000000001/0.03</f>
+        <v>3.3333333333333334E-9</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20">
+        <v>10.1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>6.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>6.45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>-6.4</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <f>0.000000892/0.04</f>
         <v>2.23E-5</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C27" s="1">
         <f>0.0000525/0.03</f>
         <v>1.75E-3</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>382.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>7.92</v>
-      </c>
-      <c r="D27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>-8.93</v>
+        <v>7.92</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
@@ -729,174 +760,188 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>-1.4</v>
+        <v>-8.93</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-1.4</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <f>0.00000192/0.03</f>
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>146.46</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>4.8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34">
-        <v>-10.4</v>
       </c>
       <c r="D34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>-10.4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>-2.9</v>
-      </c>
-      <c r="D35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>4.5999999999999996</v>
       </c>
       <c r="D36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="E39">
+        <v>50.161999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>0.15</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f>0.0000253/0.03</f>
         <v>8.433333333333333E-4</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>31</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>4.5</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41">
-        <v>-7.9</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42">
-        <v>4.5</v>
+        <v>-7.9</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43">
-        <v>-7.9</v>
+        <v>4.5</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44">
+        <v>-7.9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>0</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f>0.000000006/0.03</f>
         <v>2.0000000000000002E-7</v>
       </c>
-      <c r="D44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>7.5</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <f>0.000000019/0.03</f>
         <v>6.3333333333333345E-7</v>
       </c>
-      <c r="D45" t="s">
-        <v>16</v>
+      <c r="D46" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>